<commit_message>
removed toxicity measurement type, cleaned up Costa Rica data
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6652" uniqueCount="1495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="1494">
   <si>
     <t>HAB region</t>
   </si>
@@ -4368,9 +4368,6 @@
   </si>
   <si>
     <t>Transvector</t>
-  </si>
-  <si>
-    <t>Measurement type</t>
   </si>
   <si>
     <t>Measurement remarks</t>
@@ -5010,10 +5007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CM189"/>
+  <dimension ref="A1:CL189"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5045,55 +5042,54 @@
     <col min="30" max="30" width="22.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="24.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="41" max="51" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="15.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="15.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="26.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="7.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="5.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="7.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="17.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="7.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="19.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="21.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="21.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="13.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="17.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="19.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="90" max="91" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="92" max="16384" width="11" style="13"/>
+    <col min="36" max="36" width="19.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="40" max="50" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="15.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="16.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="26.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="7.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="21.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="21.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="13.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="17.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="19.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="17" style="13" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="17" style="13" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="18.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="17" style="13" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="89" max="90" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="91" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:91" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:90" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1066</v>
       </c>
@@ -5113,19 +5109,19 @@
       <c r="AF1" s="6" t="s">
         <v>1078</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>1084</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="AY1" s="6" t="s">
         <v>1083</v>
       </c>
-      <c r="BZ1" s="6" t="s">
+      <c r="BY1" s="6" t="s">
         <v>1109</v>
       </c>
     </row>
-    <row r="2" spans="1:91" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:90" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>0</v>
@@ -5134,7 +5130,7 @@
         <v>1067</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>1068</v>
@@ -5167,10 +5163,10 @@
         <v>1112</v>
       </c>
       <c r="S2" s="8" t="s">
+        <v>1470</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>1471</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>1472</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>1107</v>
@@ -5179,13 +5175,13 @@
         <v>1108</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>1114</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>1074</v>
@@ -5218,139 +5214,139 @@
         <v>1444</v>
       </c>
       <c r="AJ2" s="8" t="s">
+        <v>1446</v>
+      </c>
+      <c r="AN2" s="8" t="s">
+        <v>1113</v>
+      </c>
+      <c r="AO2" s="8" t="s">
+        <v>1085</v>
+      </c>
+      <c r="AP2" s="8" t="s">
+        <v>1086</v>
+      </c>
+      <c r="AQ2" s="8" t="s">
+        <v>1087</v>
+      </c>
+      <c r="AR2" s="8" t="s">
+        <v>1088</v>
+      </c>
+      <c r="AS2" s="8" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AT2" s="8" t="s">
+        <v>1090</v>
+      </c>
+      <c r="AU2" s="8" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AV2" s="8" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AW2" s="8" t="s">
+        <v>1093</v>
+      </c>
+      <c r="AX2" s="8" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AY2" s="8" t="s">
         <v>1447</v>
       </c>
-      <c r="AO2" s="8" t="s">
-        <v>1113</v>
-      </c>
-      <c r="AP2" s="8" t="s">
-        <v>1085</v>
-      </c>
-      <c r="AQ2" s="8" t="s">
-        <v>1086</v>
-      </c>
-      <c r="AR2" s="8" t="s">
-        <v>1087</v>
-      </c>
-      <c r="AS2" s="8" t="s">
-        <v>1088</v>
-      </c>
-      <c r="AT2" s="8" t="s">
-        <v>1089</v>
-      </c>
-      <c r="AU2" s="8" t="s">
-        <v>1090</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>1091</v>
-      </c>
-      <c r="AW2" s="8" t="s">
-        <v>1092</v>
-      </c>
-      <c r="AX2" s="8" t="s">
-        <v>1093</v>
-      </c>
-      <c r="AY2" s="8" t="s">
-        <v>1094</v>
-      </c>
       <c r="AZ2" s="8" t="s">
+        <v>1096</v>
+      </c>
+      <c r="BA2" s="8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="BB2" s="8" t="s">
+        <v>1449</v>
+      </c>
+      <c r="BC2" s="8" t="s">
         <v>1448</v>
       </c>
-      <c r="BA2" s="8" t="s">
-        <v>1096</v>
-      </c>
-      <c r="BB2" s="8" t="s">
-        <v>1095</v>
-      </c>
-      <c r="BC2" s="8" t="s">
+      <c r="BD2" s="8" t="s">
+        <v>1097</v>
+      </c>
+      <c r="BE2" s="8" t="s">
         <v>1450</v>
       </c>
-      <c r="BD2" s="8" t="s">
-        <v>1449</v>
-      </c>
-      <c r="BE2" s="8" t="s">
-        <v>1097</v>
-      </c>
       <c r="BF2" s="8" t="s">
+        <v>1098</v>
+      </c>
+      <c r="BG2" s="8" t="s">
         <v>1451</v>
       </c>
-      <c r="BG2" s="8" t="s">
-        <v>1098</v>
-      </c>
       <c r="BH2" s="8" t="s">
-        <v>1452</v>
+        <v>1482</v>
       </c>
       <c r="BI2" s="8" t="s">
+        <v>1099</v>
+      </c>
+      <c r="BJ2" s="8" t="s">
         <v>1483</v>
-      </c>
-      <c r="BJ2" s="8" t="s">
-        <v>1099</v>
       </c>
       <c r="BK2" s="8" t="s">
         <v>1484</v>
       </c>
       <c r="BL2" s="8" t="s">
+        <v>1404</v>
+      </c>
+      <c r="BM2" s="8" t="s">
+        <v>1100</v>
+      </c>
+      <c r="BN2" s="8" t="s">
         <v>1485</v>
       </c>
-      <c r="BM2" s="8" t="s">
-        <v>1404</v>
-      </c>
-      <c r="BN2" s="8" t="s">
-        <v>1100</v>
-      </c>
       <c r="BO2" s="8" t="s">
+        <v>1101</v>
+      </c>
+      <c r="BP2" s="8" t="s">
         <v>1486</v>
       </c>
-      <c r="BP2" s="8" t="s">
-        <v>1101</v>
-      </c>
       <c r="BQ2" s="8" t="s">
+        <v>1475</v>
+      </c>
+      <c r="BR2" s="8" t="s">
+        <v>1474</v>
+      </c>
+      <c r="BS2" s="8" t="s">
+        <v>1476</v>
+      </c>
+      <c r="BT2" s="8" t="s">
+        <v>1102</v>
+      </c>
+      <c r="BU2" s="8" t="s">
+        <v>1103</v>
+      </c>
+      <c r="BV2" s="8" t="s">
+        <v>1452</v>
+      </c>
+      <c r="BW2" s="8" t="s">
+        <v>1481</v>
+      </c>
+      <c r="BX2" s="8" t="s">
+        <v>1464</v>
+      </c>
+      <c r="BY2" s="8" t="s">
         <v>1487</v>
       </c>
-      <c r="BR2" s="8" t="s">
-        <v>1476</v>
-      </c>
-      <c r="BS2" s="8" t="s">
-        <v>1475</v>
-      </c>
-      <c r="BT2" s="8" t="s">
-        <v>1477</v>
-      </c>
-      <c r="BU2" s="8" t="s">
-        <v>1102</v>
-      </c>
-      <c r="BV2" s="8" t="s">
-        <v>1103</v>
-      </c>
-      <c r="BW2" s="8" t="s">
-        <v>1453</v>
-      </c>
-      <c r="BX2" s="8" t="s">
-        <v>1482</v>
-      </c>
-      <c r="BY2" s="8" t="s">
-        <v>1465</v>
-      </c>
-      <c r="BZ2" s="8" t="s">
-        <v>1488</v>
-      </c>
-      <c r="CB2" s="8" t="s">
+      <c r="CA2" s="8" t="s">
+        <v>1491</v>
+      </c>
+      <c r="CC2" s="10" t="s">
         <v>1492</v>
       </c>
-      <c r="CD2" s="10" t="s">
-        <v>1493</v>
-      </c>
-      <c r="CH2" s="8" t="s">
-        <v>1455</v>
+      <c r="CG2" s="8" t="s">
+        <v>1454</v>
+      </c>
+      <c r="CK2" s="8" t="s">
+        <v>1110</v>
       </c>
       <c r="CL2" s="8" t="s">
-        <v>1110</v>
-      </c>
-      <c r="CM2" s="8" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="3" spans="1:91" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:90" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E3" s="8"/>
       <c r="H3" s="11"/>
       <c r="J3" s="12" t="s">
@@ -5375,58 +5371,55 @@
         <v>1442</v>
       </c>
       <c r="AJ3" s="8" t="s">
+        <v>1111</v>
+      </c>
+      <c r="AK3" s="8" t="s">
+        <v>1115</v>
+      </c>
+      <c r="AL3" s="8" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AM3" s="8" t="s">
         <v>1445</v>
       </c>
-      <c r="AK3" s="8" t="s">
-        <v>1111</v>
-      </c>
-      <c r="AL3" s="8" t="s">
-        <v>1115</v>
-      </c>
-      <c r="AM3" s="8" t="s">
-        <v>1116</v>
-      </c>
-      <c r="AN3" s="8" t="s">
-        <v>1446</v>
+      <c r="BY3" s="8" t="s">
+        <v>1488</v>
       </c>
       <c r="BZ3" s="8" t="s">
         <v>1489</v>
       </c>
-      <c r="CA3" s="8" t="s">
-        <v>1490</v>
+      <c r="CA3" s="10" t="s">
+        <v>1488</v>
       </c>
       <c r="CB3" s="10" t="s">
         <v>1489</v>
       </c>
       <c r="CC3" s="10" t="s">
+        <v>1493</v>
+      </c>
+      <c r="CD3" s="10" t="s">
+        <v>1488</v>
+      </c>
+      <c r="CE3" s="10" t="s">
         <v>1490</v>
       </c>
-      <c r="CD3" s="10" t="s">
-        <v>1494</v>
-      </c>
-      <c r="CE3" s="10" t="s">
+      <c r="CF3" s="10" t="s">
         <v>1489</v>
       </c>
-      <c r="CF3" s="10" t="s">
-        <v>1491</v>
-      </c>
       <c r="CG3" s="10" t="s">
+        <v>1493</v>
+      </c>
+      <c r="CH3" s="10" t="s">
+        <v>1488</v>
+      </c>
+      <c r="CI3" s="10" t="s">
         <v>1490</v>
       </c>
-      <c r="CH3" s="10" t="s">
-        <v>1494</v>
-      </c>
-      <c r="CI3" s="10" t="s">
+      <c r="CJ3" s="10" t="s">
         <v>1489</v>
       </c>
-      <c r="CJ3" s="10" t="s">
-        <v>1491</v>
-      </c>
-      <c r="CK3" s="10" t="s">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="4" spans="1:91" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:90" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>1432</v>
       </c>
@@ -5533,19 +5526,19 @@
         <v>1443</v>
       </c>
       <c r="AJ4" s="21" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="AK4" s="21" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="AL4" s="21" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="AM4" s="21" t="s">
-        <v>1424</v>
-      </c>
-      <c r="AN4" s="21" t="s">
         <v>1425</v>
+      </c>
+      <c r="AN4" s="20" t="s">
+        <v>1443</v>
       </c>
       <c r="AO4" s="20" t="s">
         <v>1443</v>
@@ -5577,1395 +5570,1392 @@
       <c r="AX4" s="20" t="s">
         <v>1443</v>
       </c>
-      <c r="AY4" s="20" t="s">
+      <c r="AY4" s="21" t="s">
+        <v>1426</v>
+      </c>
+      <c r="AZ4" s="21" t="s">
+        <v>1428</v>
+      </c>
+      <c r="BA4" s="21" t="s">
+        <v>1427</v>
+      </c>
+      <c r="BB4" s="21" t="s">
+        <v>1429</v>
+      </c>
+      <c r="BC4" s="21" t="s">
+        <v>1430</v>
+      </c>
+      <c r="BD4" s="21" t="s">
+        <v>1431</v>
+      </c>
+      <c r="BE4" s="21" t="s">
+        <v>1372</v>
+      </c>
+      <c r="BF4" s="21" t="s">
+        <v>1433</v>
+      </c>
+      <c r="BG4" s="21" t="s">
+        <v>1434</v>
+      </c>
+      <c r="BH4" s="21" t="s">
+        <v>1400</v>
+      </c>
+      <c r="BI4" s="21" t="s">
+        <v>1401</v>
+      </c>
+      <c r="BJ4" s="21" t="s">
+        <v>1402</v>
+      </c>
+      <c r="BK4" s="21" t="s">
+        <v>1403</v>
+      </c>
+      <c r="BL4" s="21" t="s">
+        <v>1404</v>
+      </c>
+      <c r="BM4" s="21" t="s">
+        <v>1405</v>
+      </c>
+      <c r="BN4" s="21" t="s">
+        <v>1406</v>
+      </c>
+      <c r="BO4" s="21" t="s">
+        <v>1435</v>
+      </c>
+      <c r="BP4" s="20" t="s">
+        <v>1436</v>
+      </c>
+      <c r="BQ4" s="21" t="s">
+        <v>1407</v>
+      </c>
+      <c r="BR4" s="21" t="s">
+        <v>1438</v>
+      </c>
+      <c r="BS4" s="20" t="s">
         <v>1443</v>
       </c>
-      <c r="AZ4" s="21" t="s">
-        <v>1426</v>
-      </c>
-      <c r="BA4" s="21" t="s">
-        <v>1428</v>
-      </c>
-      <c r="BB4" s="21" t="s">
-        <v>1427</v>
-      </c>
-      <c r="BC4" s="21" t="s">
-        <v>1429</v>
-      </c>
-      <c r="BD4" s="21" t="s">
-        <v>1430</v>
-      </c>
-      <c r="BE4" s="21" t="s">
-        <v>1431</v>
-      </c>
-      <c r="BF4" s="21" t="s">
-        <v>1372</v>
-      </c>
-      <c r="BG4" s="21" t="s">
-        <v>1433</v>
-      </c>
-      <c r="BH4" s="21" t="s">
-        <v>1434</v>
-      </c>
-      <c r="BI4" s="21" t="s">
-        <v>1400</v>
-      </c>
-      <c r="BJ4" s="21" t="s">
-        <v>1401</v>
-      </c>
-      <c r="BK4" s="21" t="s">
-        <v>1402</v>
-      </c>
-      <c r="BL4" s="21" t="s">
-        <v>1403</v>
-      </c>
-      <c r="BM4" s="21" t="s">
-        <v>1404</v>
-      </c>
-      <c r="BN4" s="21" t="s">
-        <v>1405</v>
-      </c>
-      <c r="BO4" s="21" t="s">
-        <v>1406</v>
-      </c>
-      <c r="BP4" s="21" t="s">
-        <v>1435</v>
-      </c>
-      <c r="BQ4" s="20" t="s">
-        <v>1436</v>
-      </c>
-      <c r="BR4" s="21" t="s">
-        <v>1407</v>
-      </c>
-      <c r="BS4" s="21" t="s">
+      <c r="BT4" s="21" t="s">
+        <v>1408</v>
+      </c>
+      <c r="BU4" s="21" t="s">
+        <v>1437</v>
+      </c>
+      <c r="BV4" s="21" t="s">
+        <v>1409</v>
+      </c>
+      <c r="BW4" s="21" t="s">
+        <v>1420</v>
+      </c>
+      <c r="BX4" s="21" t="s">
         <v>1438</v>
       </c>
-      <c r="BT4" s="20" t="s">
-        <v>1443</v>
-      </c>
-      <c r="BU4" s="21" t="s">
-        <v>1408</v>
-      </c>
-      <c r="BV4" s="21" t="s">
-        <v>1437</v>
-      </c>
-      <c r="BW4" s="21" t="s">
-        <v>1409</v>
-      </c>
-      <c r="BX4" s="21" t="s">
-        <v>1420</v>
-      </c>
-      <c r="BY4" s="21" t="s">
+      <c r="BY4" s="20" t="s">
+        <v>1423</v>
+      </c>
+      <c r="BZ4" s="20" t="s">
+        <v>1422</v>
+      </c>
+      <c r="CA4" s="20" t="s">
+        <v>1423</v>
+      </c>
+      <c r="CB4" s="20" t="s">
+        <v>1422</v>
+      </c>
+      <c r="CC4" s="21" t="s">
+        <v>1421</v>
+      </c>
+      <c r="CD4" s="21" t="s">
+        <v>1423</v>
+      </c>
+      <c r="CE4" s="21" t="s">
+        <v>1453</v>
+      </c>
+      <c r="CF4" s="21" t="s">
+        <v>1422</v>
+      </c>
+      <c r="CG4" s="21" t="s">
+        <v>1421</v>
+      </c>
+      <c r="CH4" s="21" t="s">
+        <v>1423</v>
+      </c>
+      <c r="CI4" s="21" t="s">
+        <v>1453</v>
+      </c>
+      <c r="CJ4" s="21" t="s">
+        <v>1422</v>
+      </c>
+      <c r="CK4" s="20" t="s">
         <v>1438</v>
-      </c>
-      <c r="BZ4" s="20" t="s">
-        <v>1423</v>
-      </c>
-      <c r="CA4" s="20" t="s">
-        <v>1422</v>
-      </c>
-      <c r="CB4" s="20" t="s">
-        <v>1423</v>
-      </c>
-      <c r="CC4" s="20" t="s">
-        <v>1422</v>
-      </c>
-      <c r="CD4" s="21" t="s">
-        <v>1421</v>
-      </c>
-      <c r="CE4" s="21" t="s">
-        <v>1423</v>
-      </c>
-      <c r="CF4" s="21" t="s">
-        <v>1454</v>
-      </c>
-      <c r="CG4" s="21" t="s">
-        <v>1422</v>
-      </c>
-      <c r="CH4" s="21" t="s">
-        <v>1421</v>
-      </c>
-      <c r="CI4" s="21" t="s">
-        <v>1423</v>
-      </c>
-      <c r="CJ4" s="21" t="s">
-        <v>1454</v>
-      </c>
-      <c r="CK4" s="21" t="s">
-        <v>1422</v>
       </c>
       <c r="CL4" s="20" t="s">
         <v>1438</v>
       </c>
-      <c r="CM4" s="20" t="s">
-        <v>1438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D5" s="15"/>
+      <c r="AX5" s="18"/>
       <c r="AY5" s="18"/>
       <c r="AZ5" s="18"/>
       <c r="BA5" s="18"/>
-      <c r="BB5" s="18"/>
-    </row>
-    <row r="6" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D6" s="15"/>
+      <c r="AX6" s="18"/>
       <c r="AY6" s="18"/>
       <c r="AZ6" s="18"/>
       <c r="BA6" s="18"/>
-      <c r="BB6" s="18"/>
-    </row>
-    <row r="7" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D7" s="15"/>
+      <c r="AX7" s="18"/>
       <c r="AY7" s="18"/>
       <c r="AZ7" s="18"/>
       <c r="BA7" s="18"/>
-      <c r="BB7" s="18"/>
-    </row>
-    <row r="8" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D8" s="15"/>
+      <c r="AX8" s="18"/>
       <c r="AY8" s="18"/>
       <c r="AZ8" s="18"/>
       <c r="BA8" s="18"/>
-      <c r="BB8" s="18"/>
-    </row>
-    <row r="9" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D9" s="15"/>
+      <c r="AX9" s="18"/>
       <c r="AY9" s="18"/>
       <c r="AZ9" s="18"/>
       <c r="BA9" s="18"/>
-      <c r="BB9" s="18"/>
-    </row>
-    <row r="10" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D10" s="15"/>
+      <c r="AX10" s="18"/>
       <c r="AY10" s="18"/>
       <c r="AZ10" s="18"/>
       <c r="BA10" s="18"/>
-      <c r="BB10" s="18"/>
-    </row>
-    <row r="11" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D11" s="15"/>
+      <c r="AX11" s="18"/>
       <c r="AY11" s="18"/>
       <c r="AZ11" s="18"/>
       <c r="BA11" s="18"/>
-      <c r="BB11" s="18"/>
-    </row>
-    <row r="12" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D12" s="15"/>
+      <c r="AX12" s="18"/>
       <c r="AY12" s="18"/>
       <c r="AZ12" s="18"/>
       <c r="BA12" s="18"/>
-      <c r="BB12" s="18"/>
-    </row>
-    <row r="13" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D13" s="15"/>
+      <c r="AX13" s="18"/>
       <c r="AY13" s="18"/>
       <c r="AZ13" s="18"/>
       <c r="BA13" s="18"/>
-      <c r="BB13" s="18"/>
-    </row>
-    <row r="14" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D14" s="15"/>
+      <c r="AX14" s="18"/>
       <c r="AY14" s="18"/>
       <c r="AZ14" s="18"/>
       <c r="BA14" s="18"/>
-      <c r="BB14" s="18"/>
-    </row>
-    <row r="15" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D15" s="15"/>
+      <c r="AX15" s="18"/>
       <c r="AY15" s="18"/>
       <c r="AZ15" s="18"/>
       <c r="BA15" s="18"/>
-      <c r="BB15" s="18"/>
-    </row>
-    <row r="16" spans="1:91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:90" x14ac:dyDescent="0.2">
       <c r="D16" s="15"/>
+      <c r="AX16" s="18"/>
       <c r="AY16" s="18"/>
       <c r="AZ16" s="18"/>
       <c r="BA16" s="18"/>
-      <c r="BB16" s="18"/>
-    </row>
-    <row r="17" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D17" s="15"/>
+      <c r="AX17" s="18"/>
       <c r="AY17" s="18"/>
       <c r="AZ17" s="18"/>
       <c r="BA17" s="18"/>
-      <c r="BB17" s="18"/>
-    </row>
-    <row r="18" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D18" s="15"/>
+      <c r="AX18" s="18"/>
       <c r="AY18" s="18"/>
       <c r="AZ18" s="18"/>
       <c r="BA18" s="18"/>
-      <c r="BB18" s="18"/>
-    </row>
-    <row r="19" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D19" s="15"/>
+      <c r="AX19" s="18"/>
       <c r="AY19" s="18"/>
       <c r="AZ19" s="18"/>
       <c r="BA19" s="18"/>
-      <c r="BB19" s="18"/>
-    </row>
-    <row r="20" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D20" s="15"/>
+      <c r="AX20" s="18"/>
       <c r="AY20" s="18"/>
       <c r="AZ20" s="18"/>
       <c r="BA20" s="18"/>
-      <c r="BB20" s="18"/>
-    </row>
-    <row r="21" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D21" s="15"/>
+      <c r="AX21" s="18"/>
       <c r="AY21" s="18"/>
       <c r="AZ21" s="18"/>
       <c r="BA21" s="18"/>
-      <c r="BB21" s="18"/>
-    </row>
-    <row r="22" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D22" s="15"/>
+      <c r="AX22" s="18"/>
       <c r="AY22" s="18"/>
       <c r="AZ22" s="18"/>
       <c r="BA22" s="18"/>
-      <c r="BB22" s="18"/>
-    </row>
-    <row r="23" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D23" s="15"/>
+      <c r="AX23" s="18"/>
       <c r="AY23" s="18"/>
       <c r="AZ23" s="18"/>
       <c r="BA23" s="18"/>
-      <c r="BB23" s="18"/>
-    </row>
-    <row r="24" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D24" s="15"/>
+      <c r="AX24" s="18"/>
       <c r="AY24" s="18"/>
       <c r="AZ24" s="18"/>
       <c r="BA24" s="18"/>
-      <c r="BB24" s="18"/>
-    </row>
-    <row r="25" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D25" s="15"/>
+      <c r="AX25" s="18"/>
       <c r="AY25" s="18"/>
       <c r="AZ25" s="18"/>
       <c r="BA25" s="18"/>
-      <c r="BB25" s="18"/>
-    </row>
-    <row r="26" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D26" s="15"/>
+      <c r="AX26" s="18"/>
       <c r="AY26" s="18"/>
       <c r="AZ26" s="18"/>
       <c r="BA26" s="18"/>
-      <c r="BB26" s="18"/>
-    </row>
-    <row r="27" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D27" s="15"/>
+      <c r="AX27" s="18"/>
       <c r="AY27" s="18"/>
       <c r="AZ27" s="18"/>
       <c r="BA27" s="18"/>
-      <c r="BB27" s="18"/>
-    </row>
-    <row r="28" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D28" s="15"/>
+      <c r="AX28" s="18"/>
       <c r="AY28" s="18"/>
       <c r="AZ28" s="18"/>
       <c r="BA28" s="18"/>
-      <c r="BB28" s="18"/>
-    </row>
-    <row r="29" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D29" s="15"/>
+      <c r="AX29" s="18"/>
       <c r="AY29" s="18"/>
       <c r="AZ29" s="18"/>
       <c r="BA29" s="18"/>
-      <c r="BB29" s="18"/>
-    </row>
-    <row r="30" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D30" s="15"/>
+      <c r="AX30" s="18"/>
       <c r="AY30" s="18"/>
       <c r="AZ30" s="18"/>
       <c r="BA30" s="18"/>
-      <c r="BB30" s="18"/>
-    </row>
-    <row r="31" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D31" s="15"/>
+      <c r="AX31" s="18"/>
       <c r="AY31" s="18"/>
       <c r="AZ31" s="18"/>
       <c r="BA31" s="18"/>
-      <c r="BB31" s="18"/>
-    </row>
-    <row r="32" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D32" s="15"/>
+      <c r="AX32" s="18"/>
       <c r="AY32" s="18"/>
       <c r="AZ32" s="18"/>
       <c r="BA32" s="18"/>
-      <c r="BB32" s="18"/>
-    </row>
-    <row r="33" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D33" s="15"/>
+      <c r="AX33" s="18"/>
       <c r="AY33" s="18"/>
       <c r="AZ33" s="18"/>
       <c r="BA33" s="18"/>
-      <c r="BB33" s="18"/>
-    </row>
-    <row r="34" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D34" s="15"/>
+      <c r="AX34" s="18"/>
       <c r="AY34" s="18"/>
       <c r="AZ34" s="18"/>
       <c r="BA34" s="18"/>
-      <c r="BB34" s="18"/>
-    </row>
-    <row r="35" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D35" s="15"/>
+      <c r="AX35" s="18"/>
       <c r="AY35" s="18"/>
       <c r="AZ35" s="18"/>
       <c r="BA35" s="18"/>
-      <c r="BB35" s="18"/>
-    </row>
-    <row r="36" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D36" s="15"/>
+      <c r="AX36" s="18"/>
       <c r="AY36" s="18"/>
       <c r="AZ36" s="18"/>
       <c r="BA36" s="18"/>
-      <c r="BB36" s="18"/>
-    </row>
-    <row r="37" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D37" s="15"/>
+      <c r="AX37" s="18"/>
       <c r="AY37" s="18"/>
       <c r="AZ37" s="18"/>
       <c r="BA37" s="18"/>
-      <c r="BB37" s="18"/>
-    </row>
-    <row r="38" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D38" s="15"/>
+      <c r="AX38" s="18"/>
       <c r="AY38" s="18"/>
       <c r="AZ38" s="18"/>
       <c r="BA38" s="18"/>
-      <c r="BB38" s="18"/>
-    </row>
-    <row r="39" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D39" s="15"/>
+      <c r="AX39" s="18"/>
       <c r="AY39" s="18"/>
       <c r="AZ39" s="18"/>
       <c r="BA39" s="18"/>
-      <c r="BB39" s="18"/>
-    </row>
-    <row r="40" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D40" s="15"/>
+      <c r="AX40" s="18"/>
       <c r="AY40" s="18"/>
       <c r="AZ40" s="18"/>
       <c r="BA40" s="18"/>
-      <c r="BB40" s="18"/>
-    </row>
-    <row r="41" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D41" s="15"/>
+      <c r="AX41" s="18"/>
       <c r="AY41" s="18"/>
       <c r="AZ41" s="18"/>
       <c r="BA41" s="18"/>
-      <c r="BB41" s="18"/>
-    </row>
-    <row r="42" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D42" s="15"/>
+      <c r="AX42" s="18"/>
       <c r="AY42" s="18"/>
       <c r="AZ42" s="18"/>
       <c r="BA42" s="18"/>
-      <c r="BB42" s="18"/>
-    </row>
-    <row r="43" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D43" s="15"/>
+      <c r="AX43" s="18"/>
       <c r="AY43" s="18"/>
       <c r="AZ43" s="18"/>
       <c r="BA43" s="18"/>
-      <c r="BB43" s="18"/>
-    </row>
-    <row r="44" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D44" s="15"/>
+      <c r="AX44" s="18"/>
       <c r="AY44" s="18"/>
       <c r="AZ44" s="18"/>
       <c r="BA44" s="18"/>
-      <c r="BB44" s="18"/>
-    </row>
-    <row r="45" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D45" s="15"/>
+      <c r="AX45" s="18"/>
       <c r="AY45" s="18"/>
       <c r="AZ45" s="18"/>
       <c r="BA45" s="18"/>
-      <c r="BB45" s="18"/>
-    </row>
-    <row r="46" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D46" s="15"/>
+      <c r="AX46" s="18"/>
       <c r="AY46" s="18"/>
       <c r="AZ46" s="18"/>
       <c r="BA46" s="18"/>
-      <c r="BB46" s="18"/>
-    </row>
-    <row r="47" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D47" s="15"/>
+      <c r="AX47" s="18"/>
       <c r="AY47" s="18"/>
       <c r="AZ47" s="18"/>
       <c r="BA47" s="18"/>
-      <c r="BB47" s="18"/>
-    </row>
-    <row r="48" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D48" s="15"/>
+      <c r="AX48" s="18"/>
       <c r="AY48" s="18"/>
       <c r="AZ48" s="18"/>
       <c r="BA48" s="18"/>
-      <c r="BB48" s="18"/>
-    </row>
-    <row r="49" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D49" s="15"/>
+      <c r="AX49" s="18"/>
       <c r="AY49" s="18"/>
       <c r="AZ49" s="18"/>
       <c r="BA49" s="18"/>
-      <c r="BB49" s="18"/>
-    </row>
-    <row r="50" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D50" s="15"/>
+      <c r="AX50" s="18"/>
       <c r="AY50" s="18"/>
       <c r="AZ50" s="18"/>
       <c r="BA50" s="18"/>
-      <c r="BB50" s="18"/>
-    </row>
-    <row r="51" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D51" s="15"/>
+      <c r="AX51" s="18"/>
       <c r="AY51" s="18"/>
       <c r="AZ51" s="18"/>
       <c r="BA51" s="18"/>
-      <c r="BB51" s="18"/>
-    </row>
-    <row r="52" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D52" s="15"/>
+      <c r="AX52" s="18"/>
       <c r="AY52" s="18"/>
       <c r="AZ52" s="18"/>
       <c r="BA52" s="18"/>
-      <c r="BB52" s="18"/>
-    </row>
-    <row r="53" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D53" s="15"/>
+      <c r="AX53" s="18"/>
       <c r="AY53" s="18"/>
       <c r="AZ53" s="18"/>
       <c r="BA53" s="18"/>
-      <c r="BB53" s="18"/>
-    </row>
-    <row r="54" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D54" s="15"/>
+      <c r="AX54" s="18"/>
       <c r="AY54" s="18"/>
       <c r="AZ54" s="18"/>
       <c r="BA54" s="18"/>
-      <c r="BB54" s="18"/>
-    </row>
-    <row r="55" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D55" s="15"/>
+      <c r="AX55" s="18"/>
       <c r="AY55" s="18"/>
       <c r="AZ55" s="18"/>
       <c r="BA55" s="18"/>
-      <c r="BB55" s="18"/>
-    </row>
-    <row r="56" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D56" s="15"/>
+      <c r="AX56" s="18"/>
       <c r="AY56" s="18"/>
       <c r="AZ56" s="18"/>
       <c r="BA56" s="18"/>
-      <c r="BB56" s="18"/>
-    </row>
-    <row r="57" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D57" s="15"/>
+      <c r="AX57" s="18"/>
       <c r="AY57" s="18"/>
       <c r="AZ57" s="18"/>
       <c r="BA57" s="18"/>
-      <c r="BB57" s="18"/>
-    </row>
-    <row r="58" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D58" s="15"/>
+      <c r="AX58" s="18"/>
       <c r="AY58" s="18"/>
       <c r="AZ58" s="18"/>
       <c r="BA58" s="18"/>
-      <c r="BB58" s="18"/>
-    </row>
-    <row r="59" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D59" s="15"/>
+      <c r="AX59" s="18"/>
       <c r="AY59" s="18"/>
       <c r="AZ59" s="18"/>
       <c r="BA59" s="18"/>
-      <c r="BB59" s="18"/>
-    </row>
-    <row r="60" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D60" s="15"/>
+      <c r="AX60" s="18"/>
       <c r="AY60" s="18"/>
       <c r="AZ60" s="18"/>
       <c r="BA60" s="18"/>
-      <c r="BB60" s="18"/>
-    </row>
-    <row r="61" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D61" s="15"/>
+      <c r="AX61" s="18"/>
       <c r="AY61" s="18"/>
       <c r="AZ61" s="18"/>
       <c r="BA61" s="18"/>
-      <c r="BB61" s="18"/>
-    </row>
-    <row r="62" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D62" s="15"/>
+      <c r="AX62" s="18"/>
       <c r="AY62" s="18"/>
       <c r="AZ62" s="18"/>
       <c r="BA62" s="18"/>
-      <c r="BB62" s="18"/>
-    </row>
-    <row r="63" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D63" s="15"/>
+      <c r="AX63" s="18"/>
       <c r="AY63" s="18"/>
       <c r="AZ63" s="18"/>
       <c r="BA63" s="18"/>
-      <c r="BB63" s="18"/>
-    </row>
-    <row r="64" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D64" s="15"/>
+      <c r="AX64" s="18"/>
       <c r="AY64" s="18"/>
       <c r="AZ64" s="18"/>
       <c r="BA64" s="18"/>
-      <c r="BB64" s="18"/>
-    </row>
-    <row r="65" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D65" s="15"/>
+      <c r="AX65" s="18"/>
       <c r="AY65" s="18"/>
       <c r="AZ65" s="18"/>
       <c r="BA65" s="18"/>
-      <c r="BB65" s="18"/>
-    </row>
-    <row r="66" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D66" s="15"/>
+      <c r="AX66" s="18"/>
       <c r="AY66" s="18"/>
       <c r="AZ66" s="18"/>
       <c r="BA66" s="18"/>
-      <c r="BB66" s="18"/>
-    </row>
-    <row r="67" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D67" s="15"/>
+      <c r="AX67" s="18"/>
       <c r="AY67" s="18"/>
       <c r="AZ67" s="18"/>
       <c r="BA67" s="18"/>
-      <c r="BB67" s="18"/>
-    </row>
-    <row r="68" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D68" s="15"/>
+      <c r="AX68" s="18"/>
       <c r="AY68" s="18"/>
       <c r="AZ68" s="18"/>
       <c r="BA68" s="18"/>
-      <c r="BB68" s="18"/>
-    </row>
-    <row r="69" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D69" s="15"/>
+      <c r="AX69" s="18"/>
       <c r="AY69" s="18"/>
       <c r="AZ69" s="18"/>
       <c r="BA69" s="18"/>
-      <c r="BB69" s="18"/>
-    </row>
-    <row r="70" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D70" s="15"/>
+      <c r="AX70" s="18"/>
       <c r="AY70" s="18"/>
       <c r="AZ70" s="18"/>
       <c r="BA70" s="18"/>
-      <c r="BB70" s="18"/>
-    </row>
-    <row r="71" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D71" s="15"/>
+      <c r="AX71" s="18"/>
       <c r="AY71" s="18"/>
       <c r="AZ71" s="18"/>
       <c r="BA71" s="18"/>
-      <c r="BB71" s="18"/>
-    </row>
-    <row r="72" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D72" s="15"/>
+      <c r="AX72" s="18"/>
       <c r="AY72" s="18"/>
       <c r="AZ72" s="18"/>
       <c r="BA72" s="18"/>
-      <c r="BB72" s="18"/>
-    </row>
-    <row r="73" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D73" s="15"/>
+      <c r="AX73" s="18"/>
       <c r="AY73" s="18"/>
       <c r="AZ73" s="18"/>
       <c r="BA73" s="18"/>
-      <c r="BB73" s="18"/>
-    </row>
-    <row r="74" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D74" s="15"/>
+      <c r="AX74" s="18"/>
       <c r="AY74" s="18"/>
       <c r="AZ74" s="18"/>
       <c r="BA74" s="18"/>
-      <c r="BB74" s="18"/>
-    </row>
-    <row r="75" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D75" s="15"/>
+      <c r="AX75" s="18"/>
       <c r="AY75" s="18"/>
       <c r="AZ75" s="18"/>
       <c r="BA75" s="18"/>
-      <c r="BB75" s="18"/>
-    </row>
-    <row r="76" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D76" s="15"/>
+      <c r="AX76" s="18"/>
       <c r="AY76" s="18"/>
       <c r="AZ76" s="18"/>
       <c r="BA76" s="18"/>
-      <c r="BB76" s="18"/>
-    </row>
-    <row r="77" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D77" s="15"/>
+      <c r="AX77" s="18"/>
       <c r="AY77" s="18"/>
       <c r="AZ77" s="18"/>
       <c r="BA77" s="18"/>
-      <c r="BB77" s="18"/>
-    </row>
-    <row r="78" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D78" s="15"/>
+      <c r="AX78" s="18"/>
       <c r="AY78" s="18"/>
       <c r="AZ78" s="18"/>
       <c r="BA78" s="18"/>
-      <c r="BB78" s="18"/>
-    </row>
-    <row r="79" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D79" s="15"/>
+      <c r="AX79" s="18"/>
       <c r="AY79" s="18"/>
       <c r="AZ79" s="18"/>
       <c r="BA79" s="18"/>
-      <c r="BB79" s="18"/>
-    </row>
-    <row r="80" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D80" s="15"/>
+      <c r="AX80" s="18"/>
       <c r="AY80" s="18"/>
       <c r="AZ80" s="18"/>
       <c r="BA80" s="18"/>
-      <c r="BB80" s="18"/>
-    </row>
-    <row r="81" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D81" s="15"/>
+      <c r="AX81" s="18"/>
       <c r="AY81" s="18"/>
       <c r="AZ81" s="18"/>
       <c r="BA81" s="18"/>
-      <c r="BB81" s="18"/>
-    </row>
-    <row r="82" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D82" s="15"/>
+      <c r="AX82" s="18"/>
       <c r="AY82" s="18"/>
       <c r="AZ82" s="18"/>
       <c r="BA82" s="18"/>
-      <c r="BB82" s="18"/>
-    </row>
-    <row r="83" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D83" s="15"/>
+      <c r="AX83" s="18"/>
       <c r="AY83" s="18"/>
       <c r="AZ83" s="18"/>
       <c r="BA83" s="18"/>
-      <c r="BB83" s="18"/>
-    </row>
-    <row r="84" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D84" s="15"/>
+      <c r="AX84" s="18"/>
       <c r="AY84" s="18"/>
       <c r="AZ84" s="18"/>
       <c r="BA84" s="18"/>
-      <c r="BB84" s="18"/>
-    </row>
-    <row r="85" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D85" s="15"/>
+      <c r="AX85" s="18"/>
       <c r="AY85" s="18"/>
       <c r="AZ85" s="18"/>
       <c r="BA85" s="18"/>
-      <c r="BB85" s="18"/>
-    </row>
-    <row r="86" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D86" s="15"/>
+      <c r="AX86" s="18"/>
       <c r="AY86" s="18"/>
       <c r="AZ86" s="18"/>
       <c r="BA86" s="18"/>
-      <c r="BB86" s="18"/>
-    </row>
-    <row r="87" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D87" s="15"/>
+      <c r="AX87" s="18"/>
       <c r="AY87" s="18"/>
       <c r="AZ87" s="18"/>
       <c r="BA87" s="18"/>
-      <c r="BB87" s="18"/>
-    </row>
-    <row r="88" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D88" s="15"/>
+      <c r="AX88" s="18"/>
       <c r="AY88" s="18"/>
       <c r="AZ88" s="18"/>
       <c r="BA88" s="18"/>
-      <c r="BB88" s="18"/>
-    </row>
-    <row r="89" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D89" s="15"/>
+      <c r="AX89" s="18"/>
       <c r="AY89" s="18"/>
       <c r="AZ89" s="18"/>
       <c r="BA89" s="18"/>
-      <c r="BB89" s="18"/>
-    </row>
-    <row r="90" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D90" s="15"/>
+      <c r="AX90" s="18"/>
       <c r="AY90" s="18"/>
       <c r="AZ90" s="18"/>
       <c r="BA90" s="18"/>
-      <c r="BB90" s="18"/>
-    </row>
-    <row r="91" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D91" s="15"/>
+      <c r="AX91" s="18"/>
       <c r="AY91" s="18"/>
       <c r="AZ91" s="18"/>
       <c r="BA91" s="18"/>
-      <c r="BB91" s="18"/>
-    </row>
-    <row r="92" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D92" s="15"/>
+      <c r="AX92" s="18"/>
       <c r="AY92" s="18"/>
       <c r="AZ92" s="18"/>
       <c r="BA92" s="18"/>
-      <c r="BB92" s="18"/>
-    </row>
-    <row r="93" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D93" s="15"/>
+      <c r="AX93" s="18"/>
       <c r="AY93" s="18"/>
       <c r="AZ93" s="18"/>
       <c r="BA93" s="18"/>
-      <c r="BB93" s="18"/>
-    </row>
-    <row r="94" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D94" s="15"/>
+      <c r="AX94" s="18"/>
       <c r="AY94" s="18"/>
       <c r="AZ94" s="18"/>
       <c r="BA94" s="18"/>
-      <c r="BB94" s="18"/>
-    </row>
-    <row r="95" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D95" s="15"/>
+      <c r="AX95" s="18"/>
       <c r="AY95" s="18"/>
       <c r="AZ95" s="18"/>
       <c r="BA95" s="18"/>
-      <c r="BB95" s="18"/>
-    </row>
-    <row r="96" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D96" s="15"/>
+      <c r="AX96" s="18"/>
       <c r="AY96" s="18"/>
       <c r="AZ96" s="18"/>
       <c r="BA96" s="18"/>
-      <c r="BB96" s="18"/>
-    </row>
-    <row r="97" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D97" s="15"/>
+      <c r="AX97" s="18"/>
       <c r="AY97" s="18"/>
       <c r="AZ97" s="18"/>
       <c r="BA97" s="18"/>
-      <c r="BB97" s="18"/>
-    </row>
-    <row r="98" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D98" s="15"/>
+      <c r="AX98" s="18"/>
       <c r="AY98" s="18"/>
       <c r="AZ98" s="18"/>
       <c r="BA98" s="18"/>
-      <c r="BB98" s="18"/>
-    </row>
-    <row r="99" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D99" s="15"/>
+      <c r="AX99" s="18"/>
       <c r="AY99" s="18"/>
       <c r="AZ99" s="18"/>
       <c r="BA99" s="18"/>
-      <c r="BB99" s="18"/>
-    </row>
-    <row r="100" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D100" s="15"/>
+      <c r="AX100" s="18"/>
       <c r="AY100" s="18"/>
       <c r="AZ100" s="18"/>
       <c r="BA100" s="18"/>
-      <c r="BB100" s="18"/>
-    </row>
-    <row r="101" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D101" s="15"/>
+      <c r="AX101" s="18"/>
       <c r="AY101" s="18"/>
       <c r="AZ101" s="18"/>
       <c r="BA101" s="18"/>
-      <c r="BB101" s="18"/>
-    </row>
-    <row r="102" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D102" s="15"/>
+      <c r="AX102" s="18"/>
       <c r="AY102" s="18"/>
       <c r="AZ102" s="18"/>
       <c r="BA102" s="18"/>
-      <c r="BB102" s="18"/>
-    </row>
-    <row r="103" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D103" s="15"/>
+      <c r="AX103" s="18"/>
       <c r="AY103" s="18"/>
       <c r="AZ103" s="18"/>
       <c r="BA103" s="18"/>
-      <c r="BB103" s="18"/>
-    </row>
-    <row r="104" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D104" s="15"/>
+      <c r="AX104" s="18"/>
       <c r="AY104" s="18"/>
       <c r="AZ104" s="18"/>
       <c r="BA104" s="18"/>
-      <c r="BB104" s="18"/>
-    </row>
-    <row r="105" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D105" s="15"/>
+      <c r="AX105" s="18"/>
       <c r="AY105" s="18"/>
       <c r="AZ105" s="18"/>
       <c r="BA105" s="18"/>
-      <c r="BB105" s="18"/>
-    </row>
-    <row r="106" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D106" s="15"/>
+      <c r="AX106" s="18"/>
       <c r="AY106" s="18"/>
       <c r="AZ106" s="18"/>
       <c r="BA106" s="18"/>
-      <c r="BB106" s="18"/>
-    </row>
-    <row r="107" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D107" s="15"/>
+      <c r="AX107" s="18"/>
       <c r="AY107" s="18"/>
       <c r="AZ107" s="18"/>
       <c r="BA107" s="18"/>
-      <c r="BB107" s="18"/>
-    </row>
-    <row r="108" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D108" s="15"/>
+      <c r="AX108" s="18"/>
       <c r="AY108" s="18"/>
       <c r="AZ108" s="18"/>
       <c r="BA108" s="18"/>
-      <c r="BB108" s="18"/>
-    </row>
-    <row r="109" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D109" s="15"/>
+      <c r="AX109" s="18"/>
       <c r="AY109" s="18"/>
       <c r="AZ109" s="18"/>
       <c r="BA109" s="18"/>
-      <c r="BB109" s="18"/>
-    </row>
-    <row r="110" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D110" s="15"/>
+      <c r="AX110" s="18"/>
       <c r="AY110" s="18"/>
       <c r="AZ110" s="18"/>
       <c r="BA110" s="18"/>
-      <c r="BB110" s="18"/>
-    </row>
-    <row r="111" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D111" s="15"/>
+      <c r="AX111" s="18"/>
       <c r="AY111" s="18"/>
       <c r="AZ111" s="18"/>
       <c r="BA111" s="18"/>
-      <c r="BB111" s="18"/>
-    </row>
-    <row r="112" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D112" s="15"/>
+      <c r="AX112" s="18"/>
       <c r="AY112" s="18"/>
       <c r="AZ112" s="18"/>
       <c r="BA112" s="18"/>
-      <c r="BB112" s="18"/>
-    </row>
-    <row r="113" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D113" s="15"/>
+      <c r="AX113" s="18"/>
       <c r="AY113" s="18"/>
       <c r="AZ113" s="18"/>
       <c r="BA113" s="18"/>
-      <c r="BB113" s="18"/>
-    </row>
-    <row r="114" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D114" s="15"/>
+      <c r="AX114" s="18"/>
       <c r="AY114" s="18"/>
       <c r="AZ114" s="18"/>
       <c r="BA114" s="18"/>
-      <c r="BB114" s="18"/>
-    </row>
-    <row r="115" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D115" s="15"/>
+      <c r="AX115" s="18"/>
       <c r="AY115" s="18"/>
       <c r="AZ115" s="18"/>
       <c r="BA115" s="18"/>
-      <c r="BB115" s="18"/>
-    </row>
-    <row r="116" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D116" s="15"/>
+      <c r="AX116" s="18"/>
       <c r="AY116" s="18"/>
       <c r="AZ116" s="18"/>
       <c r="BA116" s="18"/>
-      <c r="BB116" s="18"/>
-    </row>
-    <row r="117" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D117" s="15"/>
+      <c r="AX117" s="18"/>
       <c r="AY117" s="18"/>
       <c r="AZ117" s="18"/>
       <c r="BA117" s="18"/>
-      <c r="BB117" s="18"/>
-    </row>
-    <row r="118" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D118" s="15"/>
+      <c r="AX118" s="18"/>
       <c r="AY118" s="18"/>
       <c r="AZ118" s="18"/>
       <c r="BA118" s="18"/>
-      <c r="BB118" s="18"/>
-    </row>
-    <row r="119" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D119" s="15"/>
+      <c r="AX119" s="18"/>
       <c r="AY119" s="18"/>
       <c r="AZ119" s="18"/>
       <c r="BA119" s="18"/>
-      <c r="BB119" s="18"/>
-    </row>
-    <row r="120" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D120" s="15"/>
+      <c r="AX120" s="18"/>
       <c r="AY120" s="18"/>
       <c r="AZ120" s="18"/>
       <c r="BA120" s="18"/>
-      <c r="BB120" s="18"/>
-    </row>
-    <row r="121" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D121" s="15"/>
+      <c r="AX121" s="18"/>
       <c r="AY121" s="18"/>
       <c r="AZ121" s="18"/>
       <c r="BA121" s="18"/>
-      <c r="BB121" s="18"/>
-    </row>
-    <row r="122" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D122" s="15"/>
+      <c r="AX122" s="18"/>
       <c r="AY122" s="18"/>
       <c r="AZ122" s="18"/>
       <c r="BA122" s="18"/>
-      <c r="BB122" s="18"/>
-    </row>
-    <row r="123" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D123" s="15"/>
+      <c r="AX123" s="18"/>
       <c r="AY123" s="18"/>
       <c r="AZ123" s="18"/>
       <c r="BA123" s="18"/>
-      <c r="BB123" s="18"/>
-    </row>
-    <row r="124" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D124" s="15"/>
+      <c r="AX124" s="18"/>
       <c r="AY124" s="18"/>
       <c r="AZ124" s="18"/>
       <c r="BA124" s="18"/>
-      <c r="BB124" s="18"/>
-    </row>
-    <row r="125" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D125" s="15"/>
+      <c r="AX125" s="18"/>
       <c r="AY125" s="18"/>
       <c r="AZ125" s="18"/>
       <c r="BA125" s="18"/>
-      <c r="BB125" s="18"/>
-    </row>
-    <row r="126" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D126" s="15"/>
+      <c r="AX126" s="18"/>
       <c r="AY126" s="18"/>
       <c r="AZ126" s="18"/>
       <c r="BA126" s="18"/>
-      <c r="BB126" s="18"/>
-    </row>
-    <row r="127" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D127" s="15"/>
+      <c r="AX127" s="18"/>
       <c r="AY127" s="18"/>
       <c r="AZ127" s="18"/>
       <c r="BA127" s="18"/>
-      <c r="BB127" s="18"/>
-    </row>
-    <row r="128" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D128" s="15"/>
+      <c r="AX128" s="18"/>
       <c r="AY128" s="18"/>
       <c r="AZ128" s="18"/>
       <c r="BA128" s="18"/>
-      <c r="BB128" s="18"/>
-    </row>
-    <row r="129" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D129" s="15"/>
+      <c r="AX129" s="18"/>
       <c r="AY129" s="18"/>
       <c r="AZ129" s="18"/>
       <c r="BA129" s="18"/>
-      <c r="BB129" s="18"/>
-    </row>
-    <row r="130" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D130" s="15"/>
+      <c r="AX130" s="18"/>
       <c r="AY130" s="18"/>
       <c r="AZ130" s="18"/>
       <c r="BA130" s="18"/>
-      <c r="BB130" s="18"/>
-    </row>
-    <row r="131" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D131" s="15"/>
+      <c r="AX131" s="18"/>
       <c r="AY131" s="18"/>
       <c r="AZ131" s="18"/>
       <c r="BA131" s="18"/>
-      <c r="BB131" s="18"/>
-    </row>
-    <row r="132" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D132" s="15"/>
+      <c r="AX132" s="18"/>
       <c r="AY132" s="18"/>
       <c r="AZ132" s="18"/>
       <c r="BA132" s="18"/>
-      <c r="BB132" s="18"/>
-    </row>
-    <row r="133" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D133" s="15"/>
+      <c r="AX133" s="18"/>
       <c r="AY133" s="18"/>
       <c r="AZ133" s="18"/>
       <c r="BA133" s="18"/>
-      <c r="BB133" s="18"/>
-    </row>
-    <row r="134" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D134" s="15"/>
+      <c r="AX134" s="18"/>
       <c r="AY134" s="18"/>
       <c r="AZ134" s="18"/>
       <c r="BA134" s="18"/>
-      <c r="BB134" s="18"/>
-    </row>
-    <row r="135" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D135" s="15"/>
+      <c r="AX135" s="18"/>
       <c r="AY135" s="18"/>
       <c r="AZ135" s="18"/>
       <c r="BA135" s="18"/>
-      <c r="BB135" s="18"/>
-    </row>
-    <row r="136" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D136" s="15"/>
+      <c r="AX136" s="18"/>
       <c r="AY136" s="18"/>
       <c r="AZ136" s="18"/>
       <c r="BA136" s="18"/>
-      <c r="BB136" s="18"/>
-    </row>
-    <row r="137" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D137" s="15"/>
+      <c r="AX137" s="18"/>
       <c r="AY137" s="18"/>
       <c r="AZ137" s="18"/>
       <c r="BA137" s="18"/>
-      <c r="BB137" s="18"/>
-    </row>
-    <row r="138" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D138" s="15"/>
+      <c r="AX138" s="18"/>
       <c r="AY138" s="18"/>
       <c r="AZ138" s="18"/>
       <c r="BA138" s="18"/>
-      <c r="BB138" s="18"/>
-    </row>
-    <row r="139" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D139" s="15"/>
+      <c r="AX139" s="18"/>
       <c r="AY139" s="18"/>
       <c r="AZ139" s="18"/>
       <c r="BA139" s="18"/>
-      <c r="BB139" s="18"/>
-    </row>
-    <row r="140" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D140" s="15"/>
+      <c r="AX140" s="18"/>
       <c r="AY140" s="18"/>
       <c r="AZ140" s="18"/>
       <c r="BA140" s="18"/>
-      <c r="BB140" s="18"/>
-    </row>
-    <row r="141" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D141" s="15"/>
+      <c r="AX141" s="18"/>
       <c r="AY141" s="18"/>
       <c r="AZ141" s="18"/>
       <c r="BA141" s="18"/>
-      <c r="BB141" s="18"/>
-    </row>
-    <row r="142" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D142" s="15"/>
+      <c r="AX142" s="18"/>
       <c r="AY142" s="18"/>
       <c r="AZ142" s="18"/>
       <c r="BA142" s="18"/>
-      <c r="BB142" s="18"/>
-    </row>
-    <row r="143" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D143" s="15"/>
+      <c r="AX143" s="18"/>
       <c r="AY143" s="18"/>
       <c r="AZ143" s="18"/>
       <c r="BA143" s="18"/>
-      <c r="BB143" s="18"/>
-    </row>
-    <row r="144" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D144" s="15"/>
+      <c r="AX144" s="18"/>
       <c r="AY144" s="18"/>
       <c r="AZ144" s="18"/>
       <c r="BA144" s="18"/>
-      <c r="BB144" s="18"/>
-    </row>
-    <row r="145" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D145" s="15"/>
+      <c r="AX145" s="18"/>
       <c r="AY145" s="18"/>
       <c r="AZ145" s="18"/>
       <c r="BA145" s="18"/>
-      <c r="BB145" s="18"/>
-    </row>
-    <row r="146" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D146" s="15"/>
+      <c r="AX146" s="18"/>
       <c r="AY146" s="18"/>
       <c r="AZ146" s="18"/>
       <c r="BA146" s="18"/>
-      <c r="BB146" s="18"/>
-    </row>
-    <row r="147" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D147" s="15"/>
+      <c r="AX147" s="18"/>
       <c r="AY147" s="18"/>
       <c r="AZ147" s="18"/>
       <c r="BA147" s="18"/>
-      <c r="BB147" s="18"/>
-    </row>
-    <row r="148" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D148" s="15"/>
+      <c r="AX148" s="18"/>
       <c r="AY148" s="18"/>
       <c r="AZ148" s="18"/>
       <c r="BA148" s="18"/>
-      <c r="BB148" s="18"/>
-    </row>
-    <row r="149" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D149" s="15"/>
+      <c r="AX149" s="18"/>
       <c r="AY149" s="18"/>
       <c r="AZ149" s="18"/>
       <c r="BA149" s="18"/>
-      <c r="BB149" s="18"/>
-    </row>
-    <row r="150" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D150" s="15"/>
+      <c r="AX150" s="18"/>
       <c r="AY150" s="18"/>
       <c r="AZ150" s="18"/>
       <c r="BA150" s="18"/>
-      <c r="BB150" s="18"/>
-    </row>
-    <row r="151" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D151" s="15"/>
+      <c r="AX151" s="18"/>
       <c r="AY151" s="18"/>
       <c r="AZ151" s="18"/>
       <c r="BA151" s="18"/>
-      <c r="BB151" s="18"/>
-    </row>
-    <row r="152" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D152" s="15"/>
+      <c r="AX152" s="18"/>
       <c r="AY152" s="18"/>
       <c r="AZ152" s="18"/>
       <c r="BA152" s="18"/>
-      <c r="BB152" s="18"/>
-    </row>
-    <row r="153" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D153" s="15"/>
+      <c r="AX153" s="18"/>
       <c r="AY153" s="18"/>
       <c r="AZ153" s="18"/>
       <c r="BA153" s="18"/>
-      <c r="BB153" s="18"/>
-    </row>
-    <row r="154" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D154" s="15"/>
+      <c r="AX154" s="18"/>
       <c r="AY154" s="18"/>
       <c r="AZ154" s="18"/>
       <c r="BA154" s="18"/>
-      <c r="BB154" s="18"/>
-    </row>
-    <row r="155" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D155" s="15"/>
+      <c r="AX155" s="18"/>
       <c r="AY155" s="18"/>
       <c r="AZ155" s="18"/>
       <c r="BA155" s="18"/>
-      <c r="BB155" s="18"/>
-    </row>
-    <row r="156" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D156" s="15"/>
+      <c r="AX156" s="18"/>
       <c r="AY156" s="18"/>
       <c r="AZ156" s="18"/>
       <c r="BA156" s="18"/>
-      <c r="BB156" s="18"/>
-    </row>
-    <row r="157" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D157" s="15"/>
+      <c r="AX157" s="18"/>
       <c r="AY157" s="18"/>
       <c r="AZ157" s="18"/>
       <c r="BA157" s="18"/>
-      <c r="BB157" s="18"/>
-    </row>
-    <row r="158" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D158" s="15"/>
+      <c r="AX158" s="18"/>
       <c r="AY158" s="18"/>
       <c r="AZ158" s="18"/>
       <c r="BA158" s="18"/>
-      <c r="BB158" s="18"/>
-    </row>
-    <row r="159" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D159" s="15"/>
+      <c r="AX159" s="18"/>
       <c r="AY159" s="18"/>
       <c r="AZ159" s="18"/>
       <c r="BA159" s="18"/>
-      <c r="BB159" s="18"/>
-    </row>
-    <row r="160" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D160" s="15"/>
+      <c r="AX160" s="18"/>
       <c r="AY160" s="18"/>
       <c r="AZ160" s="18"/>
       <c r="BA160" s="18"/>
-      <c r="BB160" s="18"/>
-    </row>
-    <row r="161" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D161" s="15"/>
+      <c r="AX161" s="18"/>
       <c r="AY161" s="18"/>
       <c r="AZ161" s="18"/>
       <c r="BA161" s="18"/>
-      <c r="BB161" s="18"/>
-    </row>
-    <row r="162" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D162" s="15"/>
+      <c r="AX162" s="18"/>
       <c r="AY162" s="18"/>
       <c r="AZ162" s="18"/>
       <c r="BA162" s="18"/>
-      <c r="BB162" s="18"/>
-    </row>
-    <row r="163" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D163" s="15"/>
+      <c r="AX163" s="18"/>
       <c r="AY163" s="18"/>
       <c r="AZ163" s="18"/>
       <c r="BA163" s="18"/>
-      <c r="BB163" s="18"/>
-    </row>
-    <row r="164" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="164" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D164" s="15"/>
+      <c r="AX164" s="18"/>
       <c r="AY164" s="18"/>
       <c r="AZ164" s="18"/>
       <c r="BA164" s="18"/>
-      <c r="BB164" s="18"/>
-    </row>
-    <row r="165" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="165" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D165" s="15"/>
+      <c r="AX165" s="18"/>
       <c r="AY165" s="18"/>
       <c r="AZ165" s="18"/>
       <c r="BA165" s="18"/>
-      <c r="BB165" s="18"/>
-    </row>
-    <row r="166" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="166" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D166" s="15"/>
+      <c r="AX166" s="18"/>
       <c r="AY166" s="18"/>
       <c r="AZ166" s="18"/>
       <c r="BA166" s="18"/>
-      <c r="BB166" s="18"/>
-    </row>
-    <row r="167" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="167" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D167" s="15"/>
+      <c r="AX167" s="18"/>
       <c r="AY167" s="18"/>
       <c r="AZ167" s="18"/>
       <c r="BA167" s="18"/>
-      <c r="BB167" s="18"/>
-    </row>
-    <row r="168" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="168" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D168" s="15"/>
+      <c r="AX168" s="18"/>
       <c r="AY168" s="18"/>
       <c r="AZ168" s="18"/>
       <c r="BA168" s="18"/>
-      <c r="BB168" s="18"/>
-    </row>
-    <row r="169" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="169" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D169" s="15"/>
+      <c r="AX169" s="18"/>
       <c r="AY169" s="18"/>
       <c r="AZ169" s="18"/>
       <c r="BA169" s="18"/>
-      <c r="BB169" s="18"/>
-    </row>
-    <row r="170" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="170" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D170" s="15"/>
+      <c r="AX170" s="18"/>
       <c r="AY170" s="18"/>
       <c r="AZ170" s="18"/>
       <c r="BA170" s="18"/>
-      <c r="BB170" s="18"/>
-    </row>
-    <row r="171" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="171" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D171" s="15"/>
+      <c r="AX171" s="18"/>
       <c r="AY171" s="18"/>
       <c r="AZ171" s="18"/>
       <c r="BA171" s="18"/>
-      <c r="BB171" s="18"/>
-    </row>
-    <row r="172" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="172" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D172" s="15"/>
+      <c r="AX172" s="18"/>
       <c r="AY172" s="18"/>
       <c r="AZ172" s="18"/>
       <c r="BA172" s="18"/>
-      <c r="BB172" s="18"/>
-    </row>
-    <row r="173" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="173" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D173" s="15"/>
+      <c r="AX173" s="18"/>
       <c r="AY173" s="18"/>
       <c r="AZ173" s="18"/>
       <c r="BA173" s="18"/>
-      <c r="BB173" s="18"/>
-    </row>
-    <row r="174" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="174" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D174" s="15"/>
+      <c r="AX174" s="18"/>
       <c r="AY174" s="18"/>
       <c r="AZ174" s="18"/>
       <c r="BA174" s="18"/>
-      <c r="BB174" s="18"/>
-    </row>
-    <row r="175" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D175" s="15"/>
+      <c r="AX175" s="18"/>
       <c r="AY175" s="18"/>
       <c r="AZ175" s="18"/>
       <c r="BA175" s="18"/>
-      <c r="BB175" s="18"/>
-    </row>
-    <row r="176" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="176" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D176" s="15"/>
+      <c r="AX176" s="18"/>
       <c r="AY176" s="18"/>
       <c r="AZ176" s="18"/>
       <c r="BA176" s="18"/>
-      <c r="BB176" s="18"/>
-    </row>
-    <row r="177" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="177" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D177" s="15"/>
+      <c r="AX177" s="18"/>
       <c r="AY177" s="18"/>
       <c r="AZ177" s="18"/>
       <c r="BA177" s="18"/>
-      <c r="BB177" s="18"/>
-    </row>
-    <row r="178" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="178" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D178" s="15"/>
+      <c r="AX178" s="18"/>
       <c r="AY178" s="18"/>
       <c r="AZ178" s="18"/>
       <c r="BA178" s="18"/>
-      <c r="BB178" s="18"/>
-    </row>
-    <row r="179" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="179" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D179" s="15"/>
+      <c r="AX179" s="18"/>
       <c r="AY179" s="18"/>
       <c r="AZ179" s="18"/>
       <c r="BA179" s="18"/>
-      <c r="BB179" s="18"/>
-    </row>
-    <row r="180" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="180" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D180" s="15"/>
+      <c r="AX180" s="18"/>
       <c r="AY180" s="18"/>
       <c r="AZ180" s="18"/>
       <c r="BA180" s="18"/>
-      <c r="BB180" s="18"/>
-    </row>
-    <row r="181" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="181" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D181" s="15"/>
+      <c r="AX181" s="18"/>
       <c r="AY181" s="18"/>
       <c r="AZ181" s="18"/>
       <c r="BA181" s="18"/>
-      <c r="BB181" s="18"/>
-    </row>
-    <row r="182" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="182" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D182" s="15"/>
+      <c r="AX182" s="18"/>
       <c r="AY182" s="18"/>
       <c r="AZ182" s="18"/>
       <c r="BA182" s="18"/>
-      <c r="BB182" s="18"/>
-    </row>
-    <row r="183" spans="4:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="183" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D183" s="15"/>
     </row>
-    <row r="184" spans="4:54" x14ac:dyDescent="0.2">
+    <row r="184" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D184" s="15"/>
     </row>
-    <row r="185" spans="4:54" x14ac:dyDescent="0.2">
+    <row r="185" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D185" s="15"/>
     </row>
-    <row r="186" spans="4:54" x14ac:dyDescent="0.2">
+    <row r="186" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D186" s="15"/>
     </row>
-    <row r="187" spans="4:54" x14ac:dyDescent="0.2">
+    <row r="187" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D187" s="15"/>
     </row>
-    <row r="188" spans="4:54" x14ac:dyDescent="0.2">
+    <row r="188" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D188" s="15"/>
     </row>
-    <row r="189" spans="4:54" x14ac:dyDescent="0.2">
+    <row r="189" spans="4:53" x14ac:dyDescent="0.2">
       <c r="D189" s="15"/>
     </row>
   </sheetData>
@@ -7014,13 +7004,13 @@
           <x14:formula1>
             <xm:f>lists!$C$1:$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>BS5:BS1108</xm:sqref>
+          <xm:sqref>BR5:BR1108</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lists!$D$1:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>BX5:BX1269</xm:sqref>
+          <xm:sqref>BW5:BW1269</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7044,10 +7034,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>1457</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1458</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -33182,10 +33172,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1462</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1463</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -33206,10 +33196,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -33230,7 +33220,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1383</v>
@@ -33313,43 +33303,43 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B1" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="C1" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="D1" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B2" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="C2" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="D2" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="D3" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>